<commit_message>
update IDs group 2
</commit_message>
<xml_diff>
--- a/braph2/workflows/MultiplexMRI/MultiplexMRI_examples/xls/Group2_MRI_data_layer1.xlsx
+++ b/braph2/workflows/MultiplexMRI/MultiplexMRI_examples/xls/Group2_MRI_data_layer1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kise-my.sharepoint.com/personal/anna_canal_garcia_ki_se/Documents/Dokument/GitHub/Braph-2.0-Matlab/braph2/workflows/MultiplexMRI/MultiplexMRI_examples/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_78A7DEDE8F79A8B36A3704F0FB5CC233F0A087C9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{34C54F0B-E5E1-46E3-8D0C-B713DB407F0A}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_78A7DEDE8F79A8B36A3704F0FB5CC233F0A087C9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{80B16531-F0FC-4A46-A027-087A9505E983}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="3366" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,51 +31,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>SubjectID1</t>
-  </si>
-  <si>
-    <t>label1</t>
-  </si>
-  <si>
-    <t>notes1</t>
-  </si>
-  <si>
-    <t>SubjectID2</t>
-  </si>
-  <si>
-    <t>label2</t>
-  </si>
-  <si>
-    <t>notes2</t>
-  </si>
-  <si>
-    <t>SubjectID3</t>
-  </si>
-  <si>
-    <t>label3</t>
-  </si>
-  <si>
-    <t>notes3</t>
-  </si>
-  <si>
-    <t>SubjectID4</t>
-  </si>
-  <si>
-    <t>label4</t>
-  </si>
-  <si>
-    <t>notes4</t>
-  </si>
-  <si>
-    <t>SubjectID5</t>
-  </si>
-  <si>
-    <t>label5</t>
-  </si>
-  <si>
-    <t>notes5</t>
-  </si>
-  <si>
     <t>brain region 1</t>
   </si>
   <si>
@@ -89,13 +44,58 @@
   </si>
   <si>
     <t>brain region 5</t>
+  </si>
+  <si>
+    <t>SubjectID6</t>
+  </si>
+  <si>
+    <t>SubjectID7</t>
+  </si>
+  <si>
+    <t>SubjectID8</t>
+  </si>
+  <si>
+    <t>SubjectID9</t>
+  </si>
+  <si>
+    <t>SubjectID10</t>
+  </si>
+  <si>
+    <t>label6</t>
+  </si>
+  <si>
+    <t>label7</t>
+  </si>
+  <si>
+    <t>notes6</t>
+  </si>
+  <si>
+    <t>notes7</t>
+  </si>
+  <si>
+    <t>notes8</t>
+  </si>
+  <si>
+    <t>label8</t>
+  </si>
+  <si>
+    <t>label9</t>
+  </si>
+  <si>
+    <t>notes9</t>
+  </si>
+  <si>
+    <t>notes10</t>
+  </si>
+  <si>
+    <t>label10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +107,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -501,14 +507,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.3125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="4" max="4" width="11.9453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.20703125" customWidth="1"/>
     <col min="6" max="6" width="14.62890625" customWidth="1"/>
     <col min="7" max="7" width="15.7890625" customWidth="1"/>
@@ -526,30 +532,30 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1">
         <v>0.48219269031021461</v>
@@ -569,13 +575,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1">
         <v>0.84068757026960272</v>
@@ -595,13 +601,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1">
         <v>0.21425422956179641</v>
@@ -621,13 +627,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
         <v>0.27208883310843418</v>
@@ -647,13 +653,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1">
         <v>0.58519845802667991</v>
@@ -672,6 +678,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update group 2 info xls
</commit_message>
<xml_diff>
--- a/braph2/workflows/MultiplexMRI/MultiplexMRI_examples/xls/Group2_MRI_data_layer1.xlsx
+++ b/braph2/workflows/MultiplexMRI/MultiplexMRI_examples/xls/Group2_MRI_data_layer1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kise-my.sharepoint.com/personal/anna_canal_garcia_ki_se/Documents/Dokument/GitHub/Braph-2.0-Matlab/braph2/workflows/MultiplexMRI/MultiplexMRI_examples/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_78A7DEDE8F79A8B36A3704F0FB5CC233F0A087C9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F22BFD0F-5F87-4E3B-9704-9F276E776C6B}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_78A7DEDE8F79A8B36A3704F0FB5CC233F0A087C9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB796FA7-B8DC-41A3-852F-4027E65CB022}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="366" yWindow="366" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,13 +91,13 @@
     <t>label10</t>
   </si>
   <si>
-    <t>GroupName1</t>
-  </si>
-  <si>
-    <t>TestGroup1</t>
-  </si>
-  <si>
-    <t>notes1</t>
+    <t>GroupName2</t>
+  </si>
+  <si>
+    <t>TestGroup2</t>
+  </si>
+  <si>
+    <t>notes2</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>